<commit_message>
Daily commit Confusing with expression Parser Error unsolved
</commit_message>
<xml_diff>
--- a/中间代码备忘.xlsx
+++ b/中间代码备忘.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>系统调用类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,6 +68,166 @@
   <si>
     <t>printf共有三种使用方法,因此需要使用type来分辨当前需要构造的是那种方法. 
 0-只用string 1-只用exp 2-二者兼有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>声明类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type包括int和char,最终常量存储在.data中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type包括int和char,最终变量存储在.data中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">type </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FUNC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运算类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,14 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="103" customWidth="1"/>
   </cols>
   <sheetData>
@@ -451,8 +612,165 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
daily commit tons of bugs unsolved
</commit_message>
<xml_diff>
--- a/中间代码备忘.xlsx
+++ b/中间代码备忘.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>系统调用类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,11 +147,143 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运算类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>op2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrayname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LODARR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取arrayname数组中第index个元素的值到name变量中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LODI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>END</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表征函数声明结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>FUNC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TEMP</t>
+    <t>跳转类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>func_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将一个元素取反</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -159,19 +291,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
+    <t>offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将name变量的offset位移(非数组为空)处的值设为exname的值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>label</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -179,55 +323,69 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>运算类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>op2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/</t>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GREAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LESS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EQU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_name1</t>
+  </si>
+  <si>
+    <t>exp_name1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_name2</t>
+  </si>
+  <si>
+    <t>exp_name2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_name1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -667,105 +825,318 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semi-final ver. without optimazation
</commit_message>
<xml_diff>
--- a/中间代码备忘.xlsx
+++ b/中间代码备忘.xlsx
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>